<commit_message>
small corrections are added
</commit_message>
<xml_diff>
--- a/Example_register_data.xlsx
+++ b/Example_register_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -116,6 +116,108 @@
   </si>
   <si>
     <t xml:space="preserve">dc292ebadd1d604892bde641748ee19cee62b9b0ffe4be19772d7c177567986b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEF220042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1bcb12b5317c279b350ed0b0191412635cffb5f262971755dc77fc7f7d124824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f2a96f6515d766e0c0f5ed6de3127258aa560f11711b64028016d6e48f0176d6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9cd7d16918bdc9aa37dca98ed448e21036cadcf85046b5f24c97dc8c5b937004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa002d49bb45fde0d335d886b674ecb78c6c84d98ade486d5af193e71b3c8a71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€ 58.550,29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEF220043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bdc59d6ebef908b8f0541ddc3d5f4a1772c2c49769501334193a7a0fe188775b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa0dad49d01b2866c232c18ac2e18e73a27a45e4abd3297704b9c1bb2234c629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">326718ed88d5b711d705ed98c5194002028dd00e2b1fa7f695e9d1b8ce30d29c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4e47557bdf580bc581dfe8c4978abce27041d6e3b4046f113bbedfb95abf6eb3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€ 13.400,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEF220044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95520827b63c8907da6b40938ecd8f23695ca920574d40f7475db9fd7e8e27de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">433a43012200aaa019eadbe64d9e1eb8a3a6cc8356c32e8f55d491a7b302df3b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1814aeefae6035ff65326bf2cc83c54837e7446266a0968375e35fa7220670f5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afc7a4e93efd7b7404c1eae8e3fd466f4b3f7d33db8b0302dd9f774130827a8f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€ 1.005,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEF220045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73f0a507d77a1a115b1440c951bf8a95f44dcadd56012230d6446a17ddba1849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6899293feb996b1f041ff022683838207cd08061090e50a1a208cebdfed411ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26764a93ac86121c9a6669ae5faa1f779d77e9aed107135b4b8e393c731d02dc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">964ff31e4dcd964791680c73e6d91203731d08e4d5bd73f6f13004914a8e239a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€ 59.698,34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEF220046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2f9fef92612ddba6a47095ec82726b251bcbe33855edcb520eb53b36044ba8e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7b13c29f7e0202eea2e47aade9058de6bc89b9074ee34def6405ec9ad8eb1e74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad1e0359f72c5c1a31b6057c4517eb4325ba23a348942316ec06a997a52bfca1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€ 2.010,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEF220047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f4b9bd276bdb6c2717cba9b321e4be8a96b756ca5e3ce263dae7de9256d93f32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ee2becf3bb76b185a24a905a1f4b5b25bd4bee7d033bfcaec311acfcdc86106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">753f2b620f0e036cf655b36dc868e3bb1f794d77c49f4779efeb8c4802a9919f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">974479723fcf96fce6e2468f9fa3cac2f1ce32231aed52247da6227ffe415dca</t>
   </si>
 </sst>
 </file>
@@ -236,10 +338,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,6 +473,126 @@
         <v>31</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>